<commit_message>
docs: Actualizar archivo Excel de ejemplo para pruebas de carga masiva
📄 Modificación en: ejemplo_carga_masiva_postman.xlsx
📍 Ubicación: catalogo-service/data/

🔄 Cambios:
- Se realizaron ajustes en el contenido del archivo para mejorar la claridad y utilidad en las pruebas de carga masiva.

🎯 Este archivo es utilizado en la guía de carga masiva en Postman.
</commit_message>
<xml_diff>
--- a/catalogo-service/data/ejemplo_carga_masiva_postman.xlsx
+++ b/catalogo-service/data/ejemplo_carga_masiva_postman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasibarra/uniandes/miso-uniandes/semestre4/ciclo 2/proyecto final 2/MediSupply-Backend/catalogo-service/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E6EE0-722C-1143-82CC-1209913F5017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7E1CD6-59D1-6347-9A5B-A9196550A6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,15 +61,9 @@
     <t>requiere_vencimiento</t>
   </si>
   <si>
-    <t>PROD_POSTMAN_001</t>
-  </si>
-  <si>
     <t>Amoxicilina 500mg</t>
   </si>
   <si>
-    <t>AMX500-POSTMAN</t>
-  </si>
-  <si>
     <t>ANTIBIOTICS</t>
   </si>
   <si>
@@ -85,15 +79,9 @@
     <t>true</t>
   </si>
   <si>
-    <t>PROD_POSTMAN_002</t>
-  </si>
-  <si>
     <t>Ibuprofeno 400mg</t>
   </si>
   <si>
-    <t>IBU400-POSTMAN</t>
-  </si>
-  <si>
     <t>ANALGESICS</t>
   </si>
   <si>
@@ -106,15 +94,9 @@
     <t>Temperatura ambiente</t>
   </si>
   <si>
-    <t>PROD_POSTMAN_003</t>
-  </si>
-  <si>
     <t>Losartán 50mg</t>
   </si>
   <si>
-    <t>LOS50-POSTMAN</t>
-  </si>
-  <si>
     <t>CARDIOVASCULARES</t>
   </si>
   <si>
@@ -122,6 +104,24 @@
   </si>
   <si>
     <t>Temperatura ambiente 15-25°C</t>
+  </si>
+  <si>
+    <t>PROD_POSTMAN_004</t>
+  </si>
+  <si>
+    <t>PROD_POSTMAN_005</t>
+  </si>
+  <si>
+    <t>PROD_POSTMAN_006</t>
+  </si>
+  <si>
+    <t>AMX500-POSTMAN2</t>
+  </si>
+  <si>
+    <t>IBU400-POSTMAN2</t>
+  </si>
+  <si>
+    <t>LOS50-POSTMAN2</t>
   </si>
 </sst>
 </file>
@@ -140,6 +140,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -486,11 +487,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -536,125 +543,125 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2">
+        <v>1550</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="F2">
-        <v>1250</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
       <c r="I2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K2">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3">
+        <v>850</v>
+      </c>
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <v>800</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="J3">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="K3">
         <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F4">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I4">
         <v>7</v>
       </c>
       <c r="J4">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="K4">
         <v>40</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add coverage configuration and tests for catalog and inventory routes
- Introduced .coveragerc for coverage configuration, excluding specific files and lines.
- Updated pytest.ini to set coverage fail threshold to 50 and include the new coverage config.
- Added new test files for catalog and inventory routes, enhancing test coverage with various scenarios.
- Created mock database session for unit tests to avoid dependencies on actual database.
- Included tests for bulk upload and inventory movement functionalities.
</commit_message>
<xml_diff>
--- a/catalogo-service/data/ejemplo_carga_masiva_postman.xlsx
+++ b/catalogo-service/data/ejemplo_carga_masiva_postman.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasibarra/uniandes/miso-uniandes/semestre4/ciclo 2/proyecto final 2/MediSupply-Backend/catalogo-service/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7E1CD6-59D1-6347-9A5B-A9196550A6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9B261F-F5BE-D04C-84F3-88799ADA177F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,15 +106,6 @@
     <t>Temperatura ambiente 15-25°C</t>
   </si>
   <si>
-    <t>PROD_POSTMAN_004</t>
-  </si>
-  <si>
-    <t>PROD_POSTMAN_005</t>
-  </si>
-  <si>
-    <t>PROD_POSTMAN_006</t>
-  </si>
-  <si>
     <t>AMX500-POSTMAN2</t>
   </si>
   <si>
@@ -122,6 +113,15 @@
   </si>
   <si>
     <t>LOS50-POSTMAN2</t>
+  </si>
+  <si>
+    <t>PROD_POSTMAN_009</t>
+  </si>
+  <si>
+    <t>PROD_POSTMAN_010</t>
+  </si>
+  <si>
+    <t>PROD_POSTMAN_012</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -543,13 +543,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -584,13 +584,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -625,13 +625,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>

</xml_diff>